<commit_message>
ADD : IMAP mail AND initAllApp fonctionne
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Calmettes\Documents\UiPath\GmailEmailManagement\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74DB724-A66F-4B04-A65B-0E4AC92EABE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C81A807-8AAE-481A-9C9F-E47A96BD7A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-  </si>
-  <si>
     <t>GmailEmail</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>mdpMail</t>
+  </si>
+  <si>
+    <t>EmailInformationQueue</t>
   </si>
 </sst>
 </file>
@@ -550,15 +550,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.53125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.46484375" customWidth="1"/>
+    <col min="4" max="26" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -600,13 +600,13 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="42.75">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -616,7 +616,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="28.5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -629,18 +629,18 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1649,12 +1649,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.46484375" customWidth="1"/>
+    <col min="4" max="26" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1691,7 +1691,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="28.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1816,7 +1816,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="28.5">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2810,12 +2810,12 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.9296875" customWidth="1"/>
+    <col min="2" max="2" width="30.06640625" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>